<commit_message>
Upload changed from product name to product_id
</commit_message>
<xml_diff>
--- a/public/excel-import-template.xlsx
+++ b/public/excel-import-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t xml:space="preserve">month</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">mobile_no</t>
   </si>
   <si>
-    <t xml:space="preserve">product_name</t>
+    <t xml:space="preserve">product_id</t>
   </si>
   <si>
     <t xml:space="preserve">attribute</t>
@@ -82,13 +82,7 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
-    <t xml:space="preserve">BISLERI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyz</t>
   </si>
 </sst>
 </file>
@@ -205,10 +199,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="M1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.48"/>
@@ -307,11 +301,11 @@
       <c r="K2" s="0" t="n">
         <v>8377040768</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>100</v>
@@ -354,11 +348,11 @@
       <c r="K3" s="0" t="n">
         <v>8377040768</v>
       </c>
-      <c r="L3" s="0" t="s">
-        <v>22</v>
+      <c r="L3" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>100</v>

</xml_diff>

<commit_message>
Multiple invoice id created
</commit_message>
<xml_diff>
--- a/public/excel-import-template.xlsx
+++ b/public/excel-import-template.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
   <si>
     <t xml:space="preserve">month</t>
   </si>
@@ -55,6 +58,9 @@
     <t xml:space="preserve">mobile_no</t>
   </si>
   <si>
+    <t xml:space="preserve">email_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">product_id</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
     <t xml:space="preserve">quantity</t>
   </si>
   <si>
+    <t xml:space="preserve">30-12-2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">December</t>
   </si>
   <si>
@@ -82,7 +91,13 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
+    <t xml:space="preserve">adnanhmd000@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31-12-2022</t>
   </si>
 </sst>
 </file>
@@ -92,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -120,6 +135,24 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -173,7 +206,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,25 +241,25 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="89.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="55.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="89.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="55.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,7 +299,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -263,105 +308,125 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>8377040768</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="D3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="I3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>8377040768</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="0" t="n">
+      <c r="M3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="O2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>8377040768</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="Q3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" display="adnanhmd000@gmail.com"/>
+    <hyperlink ref="M3" r:id="rId2" display="adnanhmd000@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>